<commit_message>
Pulling from cleaned.csv.  Functional.  Tweaking for flowthrough data.
</commit_message>
<xml_diff>
--- a/Sentiment Engines/Date Time Cleaning/test formats.xlsx
+++ b/Sentiment Engines/Date Time Cleaning/test formats.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\Ubiqum Data Science\project\Sentiment Engines\Date Time Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="5610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="5610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test formats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="178">
   <si>
     <t>articleTime</t>
   </si>
@@ -376,12 +376,193 @@
   </si>
   <si>
     <t>2017-12-01 12:21</t>
+  </si>
+  <si>
+    <t>_x000D_
+       _x000D_
+           4 Dec 2017</t>
+  </si>
+  <si>
+    <t>_x000D_
+       _x000D_
+           6 Dec 2017</t>
+  </si>
+  <si>
+    <t>1 month ago</t>
+  </si>
+  <si>
+    <t>7 minutes ago</t>
+  </si>
+  <si>
+    <t>3 hours ago</t>
+  </si>
+  <si>
+    <t>2 days ago</t>
+  </si>
+  <si>
+    <t>13 minutes ago</t>
+  </si>
+  <si>
+    <t>8 minutes ago</t>
+  </si>
+  <si>
+    <t>Redit BTC Bay</t>
+  </si>
+  <si>
+    <t>Redit BTC Markets</t>
+  </si>
+  <si>
+    <t>5 hours ago</t>
+  </si>
+  <si>
+    <t>10 hours ago</t>
+  </si>
+  <si>
+    <t>4 hours ago</t>
+  </si>
+  <si>
+    <t>20 hours ago</t>
+  </si>
+  <si>
+    <t>18 hours ago</t>
+  </si>
+  <si>
+    <t>9 minutes ago</t>
+  </si>
+  <si>
+    <t>14 minutes ago</t>
+  </si>
+  <si>
+    <t>3 minutes ago</t>
+  </si>
+  <si>
+    <t>4 minutes ago</t>
+  </si>
+  <si>
+    <t>18 minutes ago</t>
+  </si>
+  <si>
+    <t>Redit BTC Mining</t>
+  </si>
+  <si>
+    <t>6 hours ago</t>
+  </si>
+  <si>
+    <t>12 minutes ago</t>
+  </si>
+  <si>
+    <t>42 minutes ago</t>
+  </si>
+  <si>
+    <t>36 minutes ago</t>
+  </si>
+  <si>
+    <t>Redit Crypto</t>
+  </si>
+  <si>
+    <t>5 min ago</t>
+  </si>
+  <si>
+    <t>14 min ago</t>
+  </si>
+  <si>
+    <t>19 hours ago</t>
+  </si>
+  <si>
+    <t>Jan. 3, 2018 5:40 am ET</t>
+  </si>
+  <si>
+    <t>Jan. 3, 2018 3:40 am ET</t>
+  </si>
+  <si>
+    <t>Jan. 2, 2018 4:51 pm ET</t>
+  </si>
+  <si>
+    <t>Jan. 2, 2018 1:23 pm ET</t>
+  </si>
+  <si>
+    <t>Wall Street Journal</t>
+  </si>
+  <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>19m</t>
+  </si>
+  <si>
+    <t>24m</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>33m</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>Google Plus</t>
+  </si>
+  <si>
+    <t>Bloomberg</t>
+  </si>
+  <si>
+    <t>Dec 15,2017.... The laborious creation of each digital Bitcoin has real-world consequences.</t>
+  </si>
+  <si>
+    <t>Dec 15,2017.... Despite glitzy tech breakthroughs, the U.S. is getting less bang for its R&amp;amp;D buck. Hereâ€™s what i...</t>
+  </si>
+  <si>
+    <t>Dec 16,2017.... This is your Cyber Saturday edition of Fortune's tech newsletter for December 16, 2017.</t>
+  </si>
+  <si>
+    <t>Dec 18,2017.... CME Group, the world's largest derivatives exchange operator, has begun trading bitcoin futures.</t>
+  </si>
+  <si>
+    <t>Dec 17,2017.... The infamous North Korean hacking outfit, Lazarus Group, is running a spear-phishing campaign aimed ...</t>
+  </si>
+  <si>
+    <t>Fortune</t>
+  </si>
+  <si>
+    <t>5 days ago</t>
+  </si>
+  <si>
+    <t>7 hours ago</t>
+  </si>
+  <si>
+    <t>5 minutes ago</t>
+  </si>
+  <si>
+    <t>Redit BTC XT</t>
+  </si>
+  <si>
+    <t>13/12/2017</t>
+  </si>
+  <si>
+    <t>15/12/2017</t>
+  </si>
+  <si>
+    <t>14/12/2017</t>
+  </si>
+  <si>
+    <t>Crypto Coin News</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -888,7 +1069,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -917,6 +1098,12 @@
     <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1271,16 +1458,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="105" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.86328125" style="6" customWidth="1"/>
     <col min="2" max="2" width="22.1328125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.53125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.06640625" style="6"/>
@@ -1326,8 +1513,8 @@
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>112</v>
+      <c r="C4">
+        <v>43068.807962962899</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1348,8 +1535,8 @@
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>99</v>
+      <c r="C6" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -1359,8 +1546,8 @@
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>100</v>
+      <c r="C7" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1371,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1382,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1392,8 +1579,8 @@
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>103</v>
+      <c r="C10" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -1404,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1412,10 +1599,10 @@
         <v>113</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>115</v>
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1426,7 +1613,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1437,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1448,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -1456,10 +1643,10 @@
         <v>113</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -1470,7 +1657,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -1481,7 +1668,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -1492,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -1503,7 +1690,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -1514,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -1525,7 +1712,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -1536,7 +1723,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -1547,7 +1734,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1558,7 +1745,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -1569,7 +1756,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -1580,7 +1767,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -1591,7 +1778,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -1609,11 +1796,11 @@
       <c r="A30" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>21</v>
+      <c r="B30" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -1624,7 +1811,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
@@ -1635,7 +1822,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
@@ -1646,7 +1833,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
@@ -1657,7 +1844,7 @@
         <v>21</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
@@ -1668,7 +1855,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
@@ -1679,7 +1866,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
@@ -1690,18 +1877,18 @@
         <v>21</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>30</v>
+      <c r="B38" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
@@ -1712,7 +1899,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
@@ -1723,7 +1910,7 @@
         <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -1734,7 +1921,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
@@ -1745,7 +1932,7 @@
         <v>30</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -1756,7 +1943,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -1767,7 +1954,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -1778,29 +1965,29 @@
         <v>30</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>29</v>
+      <c r="C46" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>38</v>
+      <c r="B47" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -1811,7 +1998,7 @@
         <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -1822,7 +2009,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
@@ -1830,10 +2017,10 @@
         <v>113</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
@@ -1844,7 +2031,7 @@
         <v>43</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
@@ -1855,7 +2042,7 @@
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -1866,18 +2053,18 @@
         <v>43</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>47</v>
+      <c r="B54" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -1888,7 +2075,7 @@
         <v>47</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
@@ -1899,7 +2086,7 @@
         <v>47</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
@@ -1910,7 +2097,7 @@
         <v>47</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -1921,7 +2108,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -1932,7 +2119,7 @@
         <v>47</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -1943,7 +2130,7 @@
         <v>47</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -1954,7 +2141,7 @@
         <v>47</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -1962,10 +2149,10 @@
         <v>113</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -1976,7 +2163,7 @@
         <v>49</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
@@ -1987,18 +2174,18 @@
         <v>49</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>53</v>
+      <c r="B65" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
@@ -2009,7 +2196,7 @@
         <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
@@ -2020,7 +2207,7 @@
         <v>53</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
@@ -2031,7 +2218,7 @@
         <v>53</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
@@ -2042,7 +2229,7 @@
         <v>53</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
@@ -2064,7 +2251,7 @@
         <v>53</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -2075,7 +2262,7 @@
         <v>53</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -2086,18 +2273,18 @@
         <v>53</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>62</v>
+      <c r="B74" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
@@ -2108,7 +2295,7 @@
         <v>62</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -2119,29 +2306,29 @@
         <v>62</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>65</v>
+      <c r="C77" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>66</v>
+      <c r="B78" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -2152,7 +2339,7 @@
         <v>67</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
@@ -2163,18 +2350,18 @@
         <v>67</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>70</v>
+      <c r="C81" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
@@ -2185,7 +2372,7 @@
         <v>67</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -2196,18 +2383,18 @@
         <v>67</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>73</v>
+      <c r="B84" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
@@ -2218,7 +2405,7 @@
         <v>74</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
@@ -2229,7 +2416,7 @@
         <v>74</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
@@ -2240,29 +2427,29 @@
         <v>74</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>78</v>
+      <c r="B89" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -2273,7 +2460,7 @@
         <v>78</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
@@ -2284,7 +2471,7 @@
         <v>78</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
@@ -2295,29 +2482,29 @@
         <v>78</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>82</v>
+      <c r="C93" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>83</v>
+      <c r="B94" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
@@ -2328,7 +2515,7 @@
         <v>84</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
@@ -2339,7 +2526,7 @@
         <v>84</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
@@ -2350,7 +2537,7 @@
         <v>84</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
@@ -2361,7 +2548,7 @@
         <v>84</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
@@ -2372,7 +2559,7 @@
         <v>84</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
@@ -2383,7 +2570,7 @@
         <v>84</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
@@ -2394,7 +2581,7 @@
         <v>84</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
@@ -2405,7 +2592,7 @@
         <v>84</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
@@ -2416,7 +2603,7 @@
         <v>84</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
@@ -2427,7 +2614,7 @@
         <v>84</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
@@ -2438,18 +2625,18 @@
         <v>84</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
@@ -2457,21 +2644,1385 @@
         <v>113</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C109" s="4" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A112" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A113" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>127</v>
+      </c>
+      <c r="C114" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>127</v>
+      </c>
+      <c r="C115" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B116" t="s">
+        <v>127</v>
+      </c>
+      <c r="C116" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" t="s">
+        <v>127</v>
+      </c>
+      <c r="C117" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B118" t="s">
+        <v>127</v>
+      </c>
+      <c r="C118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B119" t="s">
+        <v>127</v>
+      </c>
+      <c r="C119" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B120" t="s">
+        <v>127</v>
+      </c>
+      <c r="C120" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B121" t="s">
+        <v>127</v>
+      </c>
+      <c r="C121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A122" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B122" t="s">
+        <v>127</v>
+      </c>
+      <c r="C122" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A123" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B123" t="s">
+        <v>127</v>
+      </c>
+      <c r="C123" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A124" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B124" t="s">
+        <v>127</v>
+      </c>
+      <c r="C124" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A125" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B125" t="s">
+        <v>127</v>
+      </c>
+      <c r="C125" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A126" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B126" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A127" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B127" t="s">
+        <v>127</v>
+      </c>
+      <c r="C127" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A128" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" t="s">
+        <v>127</v>
+      </c>
+      <c r="C128" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A129" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A130" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130" t="s">
+        <v>128</v>
+      </c>
+      <c r="C130" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A131" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B131" t="s">
+        <v>128</v>
+      </c>
+      <c r="C131" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A132" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B132" t="s">
+        <v>128</v>
+      </c>
+      <c r="C132" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A133" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B133" t="s">
+        <v>128</v>
+      </c>
+      <c r="C133" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A134" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B134" t="s">
+        <v>128</v>
+      </c>
+      <c r="C134" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A135" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B135" t="s">
+        <v>128</v>
+      </c>
+      <c r="C135" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B136" t="s">
+        <v>128</v>
+      </c>
+      <c r="C136" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B137" t="s">
+        <v>128</v>
+      </c>
+      <c r="C137" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B138" t="s">
+        <v>128</v>
+      </c>
+      <c r="C138" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B139" t="s">
+        <v>128</v>
+      </c>
+      <c r="C139" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B140" t="s">
+        <v>128</v>
+      </c>
+      <c r="C140" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B141" t="s">
+        <v>128</v>
+      </c>
+      <c r="C141" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B142" t="s">
+        <v>128</v>
+      </c>
+      <c r="C142" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A143" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B143" t="s">
+        <v>128</v>
+      </c>
+      <c r="C143" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A144" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B144" t="s">
+        <v>128</v>
+      </c>
+      <c r="C144" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A145" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B145" t="s">
+        <v>128</v>
+      </c>
+      <c r="C145" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A146" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B146" t="s">
+        <v>128</v>
+      </c>
+      <c r="C146" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A147" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B147" t="s">
+        <v>128</v>
+      </c>
+      <c r="C147" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A148" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B148" t="s">
+        <v>128</v>
+      </c>
+      <c r="C148" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A149" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B149" t="s">
+        <v>128</v>
+      </c>
+      <c r="C149" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A150" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B150" t="s">
+        <v>128</v>
+      </c>
+      <c r="C150" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A151" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B151" t="s">
+        <v>128</v>
+      </c>
+      <c r="C151" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A152" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B152" t="s">
+        <v>128</v>
+      </c>
+      <c r="C152" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A153" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B153" t="s">
+        <v>128</v>
+      </c>
+      <c r="C153" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A154" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B154" t="s">
+        <v>128</v>
+      </c>
+      <c r="C154" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A155" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B155" t="s">
+        <v>128</v>
+      </c>
+      <c r="C155" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A156" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B156" t="s">
+        <v>128</v>
+      </c>
+      <c r="C156" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A157" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B157" t="s">
+        <v>128</v>
+      </c>
+      <c r="C157" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A158" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B158" t="s">
+        <v>128</v>
+      </c>
+      <c r="C158" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A159" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B159" t="s">
+        <v>128</v>
+      </c>
+      <c r="C159" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A160" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B160" t="s">
+        <v>128</v>
+      </c>
+      <c r="C160" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A161" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B161" t="s">
+        <v>128</v>
+      </c>
+      <c r="C161" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A162" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B162" t="s">
+        <v>128</v>
+      </c>
+      <c r="C162" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A163" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B163" t="s">
+        <v>128</v>
+      </c>
+      <c r="C163" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A164" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B164" t="s">
+        <v>128</v>
+      </c>
+      <c r="C164" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A165" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B165" t="s">
+        <v>128</v>
+      </c>
+      <c r="C165" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A166" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B166" t="s">
+        <v>128</v>
+      </c>
+      <c r="C166" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A167" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B167" t="s">
+        <v>128</v>
+      </c>
+      <c r="C167" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A168" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B168" t="s">
+        <v>128</v>
+      </c>
+      <c r="C168" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A169" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B169" t="s">
+        <v>139</v>
+      </c>
+      <c r="C169" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A170" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B170" t="s">
+        <v>139</v>
+      </c>
+      <c r="C170" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A171" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B171" t="s">
+        <v>139</v>
+      </c>
+      <c r="C171" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A172" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B172" t="s">
+        <v>139</v>
+      </c>
+      <c r="C172" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A173" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B173" t="s">
+        <v>139</v>
+      </c>
+      <c r="C173" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A174" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B174" t="s">
+        <v>139</v>
+      </c>
+      <c r="C174" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A175" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B175" t="s">
+        <v>139</v>
+      </c>
+      <c r="C175" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A176" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B176" t="s">
+        <v>139</v>
+      </c>
+      <c r="C176" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A177" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B177" t="s">
+        <v>139</v>
+      </c>
+      <c r="C177" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A178" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B178" t="s">
+        <v>139</v>
+      </c>
+      <c r="C178" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A179" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B179" t="s">
+        <v>139</v>
+      </c>
+      <c r="C179" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A180" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B180" t="s">
+        <v>139</v>
+      </c>
+      <c r="C180" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A181" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B181" t="s">
+        <v>139</v>
+      </c>
+      <c r="C181" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A182" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B182" t="s">
+        <v>139</v>
+      </c>
+      <c r="C182" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A183" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B183" t="s">
+        <v>139</v>
+      </c>
+      <c r="C183" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A184" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B184" t="s">
+        <v>139</v>
+      </c>
+      <c r="C184" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A185" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B185" t="s">
+        <v>139</v>
+      </c>
+      <c r="C185" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A186" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B186" t="s">
+        <v>144</v>
+      </c>
+      <c r="C186" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A187" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B187" t="s">
+        <v>144</v>
+      </c>
+      <c r="C187" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A188" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B188" t="s">
+        <v>144</v>
+      </c>
+      <c r="C188" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A189" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B189" t="s">
+        <v>144</v>
+      </c>
+      <c r="C189" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A190" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B190" t="s">
+        <v>144</v>
+      </c>
+      <c r="C190" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A191" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B191" t="s">
+        <v>144</v>
+      </c>
+      <c r="C191" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A192" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B192" t="s">
+        <v>144</v>
+      </c>
+      <c r="C192" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A193" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B193" t="s">
+        <v>144</v>
+      </c>
+      <c r="C193" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A194" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B194" t="s">
+        <v>144</v>
+      </c>
+      <c r="C194" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A195" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B195" t="s">
+        <v>144</v>
+      </c>
+      <c r="C195" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A196" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B196" t="s">
+        <v>144</v>
+      </c>
+      <c r="C196" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A197" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B197" t="s">
+        <v>152</v>
+      </c>
+      <c r="C197" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A198" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B198" t="s">
+        <v>152</v>
+      </c>
+      <c r="C198" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A199" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B199" t="s">
+        <v>152</v>
+      </c>
+      <c r="C199" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A200" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B200" t="s">
+        <v>152</v>
+      </c>
+      <c r="C200" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A201" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B201" t="s">
+        <v>152</v>
+      </c>
+      <c r="C201" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A202" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B202" t="s">
+        <v>152</v>
+      </c>
+      <c r="C202" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A203" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B203" t="s">
+        <v>152</v>
+      </c>
+      <c r="C203" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A204" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B204" t="s">
+        <v>152</v>
+      </c>
+      <c r="C204" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A205" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B205" t="s">
+        <v>152</v>
+      </c>
+      <c r="C205" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A206" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C206" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A207" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C207" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A208" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C208" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A209" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C209" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A210" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C210" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A211" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C211" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A212" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C212" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A213" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C213" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A214" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C214" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A215" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C215" s="13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A216" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B216" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C216" s="14">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A217" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B217" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C217" s="15">
+        <v>0.74375000000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A218" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A219" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A220" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A221" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B221" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A222" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C222" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A223" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B223" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C223" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A224" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C224" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A225" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C225" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A226" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A227" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C227" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A228" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B228" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C228" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A229" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C229" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A230" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C230" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A231" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C231" s="13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A232" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C232" s="13" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>